<commit_message>
optimize the UI by python ,update the profit
</commit_message>
<xml_diff>
--- a/py/data.xlsx
+++ b/py/data.xlsx
@@ -82,9 +82,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -387,10 +388,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C39"/>
+  <dimension ref="A1:D42"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A34" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C41" sqref="C41"/>
+      <selection activeCell="D44" sqref="D44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -576,7 +577,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A17">
         <v>0</v>
       </c>
@@ -587,7 +588,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A18">
         <v>0</v>
       </c>
@@ -598,7 +599,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A19">
         <v>0</v>
       </c>
@@ -609,7 +610,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A20">
         <v>0</v>
       </c>
@@ -620,7 +621,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A21">
         <v>0</v>
       </c>
@@ -631,7 +632,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A22">
         <v>0</v>
       </c>
@@ -642,7 +643,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A23">
         <v>0</v>
       </c>
@@ -653,7 +654,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A24">
         <v>0</v>
       </c>
@@ -664,7 +665,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A25">
         <v>0</v>
       </c>
@@ -675,7 +676,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A26">
         <v>0</v>
       </c>
@@ -686,7 +687,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A27">
         <v>0</v>
       </c>
@@ -697,7 +698,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A28">
         <v>0</v>
       </c>
@@ -708,7 +709,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A29">
         <v>0</v>
       </c>
@@ -719,7 +720,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A30">
         <v>0</v>
       </c>
@@ -730,7 +731,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A31">
         <v>0</v>
       </c>
@@ -740,8 +741,11 @@
       <c r="C31">
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D31">
+        <v>17000</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A32">
         <v>-0.7</v>
       </c>
@@ -752,7 +756,7 @@
         <v>7.4999999999999997E-3</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A33">
         <v>-0.24199999999999999</v>
       </c>
@@ -763,7 +767,7 @@
         <v>3.5299999999999998E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A34">
         <v>0.63100000000000001</v>
       </c>
@@ -774,7 +778,7 @@
         <v>9.9000000000000008E-3</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A35">
         <v>0.71</v>
       </c>
@@ -785,7 +789,7 @@
         <v>5.4100000000000002E-2</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A36">
         <v>0.37</v>
       </c>
@@ -796,7 +800,7 @@
         <v>3.6799999999999999E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A37">
         <v>0.54</v>
       </c>
@@ -807,7 +811,7 @@
         <v>4.4200000000000003E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A38">
         <v>0.44</v>
       </c>
@@ -819,7 +823,7 @@
         <v>2.53E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A39">
         <v>0.6</v>
       </c>
@@ -828,10 +832,48 @@
       </c>
       <c r="C39" s="1">
         <v>4.3499999999999997E-2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A40">
+        <v>0.09</v>
+      </c>
+      <c r="B40" s="2">
+        <v>0.96</v>
+      </c>
+      <c r="C40" s="1">
+        <v>1.12E-2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A41">
+        <v>0.2</v>
+      </c>
+      <c r="B41" s="2">
+        <v>0.95</v>
+      </c>
+      <c r="C41" s="1">
+        <v>2.6700000000000002E-2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A42">
+        <v>0.11</v>
+      </c>
+      <c r="B42" s="2">
+        <v>0.95</v>
+      </c>
+      <c r="C42" s="1">
+        <f>(D42-D31)/D31</f>
+        <v>0.11</v>
+      </c>
+      <c r="D42">
+        <v>18870</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add the prediction strategy
</commit_message>
<xml_diff>
--- a/py/data.xlsx
+++ b/py/data.xlsx
@@ -85,7 +85,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -388,10 +388,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D43"/>
+  <dimension ref="A1:D48"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A31" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="D44" sqref="D44"/>
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -747,7 +747,7 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A32">
-        <v>-0.7</v>
+        <v>0</v>
       </c>
       <c r="B32">
         <v>0.98</v>
@@ -758,7 +758,7 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A33">
-        <v>-0.24199999999999999</v>
+        <v>0</v>
       </c>
       <c r="B33">
         <v>0.98</v>
@@ -875,7 +875,7 @@
       <c r="A43">
         <v>0.14000000000000001</v>
       </c>
-      <c r="B43" s="1">
+      <c r="B43" s="2">
         <v>0.98799999999999999</v>
       </c>
       <c r="C43" s="1">
@@ -883,6 +883,84 @@
       </c>
       <c r="D43">
         <v>19010</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A44">
+        <v>0.06</v>
+      </c>
+      <c r="B44" s="2">
+        <v>0.89</v>
+      </c>
+      <c r="C44" s="1">
+        <v>0.1095</v>
+      </c>
+      <c r="D44">
+        <v>18861</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A45">
+        <v>0.16</v>
+      </c>
+      <c r="B45">
+        <f>18207/19983</f>
+        <v>0.91112445578741896</v>
+      </c>
+      <c r="C45">
+        <f>(19983-17000)/17000</f>
+        <v>0.17547058823529399</v>
+      </c>
+      <c r="D45">
+        <v>19983</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A46">
+        <v>0.42</v>
+      </c>
+      <c r="B46">
+        <f>17586/D46</f>
+        <v>0.908227030935289</v>
+      </c>
+      <c r="C46">
+        <f>(D46-D31)/D31</f>
+        <v>0.13900000000000001</v>
+      </c>
+      <c r="D46">
+        <v>19363</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A47">
+        <v>0.59</v>
+      </c>
+      <c r="B47">
+        <f>17937/D47</f>
+        <v>0.88841010401188703</v>
+      </c>
+      <c r="C47">
+        <f>(D47-D31)/D31</f>
+        <v>0.187647058823529</v>
+      </c>
+      <c r="D47">
+        <v>20190</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A48">
+        <v>0.1</v>
+      </c>
+      <c r="B48">
+        <f>18810/D48</f>
+        <v>0.94884987893462502</v>
+      </c>
+      <c r="C48">
+        <f>(D48-D31)/D31</f>
+        <v>0.16611764705882401</v>
+      </c>
+      <c r="D48">
+        <v>19824</v>
       </c>
     </row>
   </sheetData>

</xml_diff>